<commit_message>
Finished convert all variables from pyllelic to pyllelic_cpg
</commit_message>
<xml_diff>
--- a/Test1_diff.xlsx
+++ b/Test1_diff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:BH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,137 +436,297 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>1293588</t>
+          <t>AAAAACACACAACATCACAAAAATAACCA</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>1293690</t>
+          <t>AAAAACGCGCGACATCGCGAAAATAACCG</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>1293730</t>
+          <t>AACACTACCCCCGCGCCTCCTCGCACCCG</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>1294031</t>
+          <t>AACCAAACGCTCCTACTAACCGCGCACCG</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1294196</t>
+          <t>AACCACAACAACCTTAACCCTAAACCCCG</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>1294262</t>
+          <t>AACCACAACGACCTTAACCCTAAACCCCG</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>1294316</t>
+          <t>AACCTAACCCCGACAACGCAACTACTCCG</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>1294369</t>
+          <t>ACCACCACAAAACCCTAAAACTTCTCCCG</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>1294419</t>
+          <t>ACCACCCCAAATCTATTAATCACCCACCG</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>1294872</t>
+          <t>ACCGCCACAAAACCCTAAAACTTCTCCCG</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>1294945</t>
+          <t>ACCGCCACAAAACCCTAAAACTTCTCCNG</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>1294972</t>
+          <t>ACGATCACTCGATCCACGCGTCCTACCCG</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>1295089</t>
+          <t>CGAAATCCACTAACGTATAACGAAAACCG</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>1295116</t>
+          <t>CGGACGTGAAGGGGAGGACGGAGGCGCGT</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>1295246</t>
+          <t>CGGAGTGTTTTTTTGTAATATTTTTTCGC</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>1295320</t>
+          <t>CGGCGTAGGTAGGTTCGTACGAAGTCGTA</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>1295365</t>
+          <t>CGGCGTAGGTAGGTTCGTACGAAGTTGTA</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>1295393</t>
+          <t>CGGCGTAGGTAGGTTCGTATGAAGTCGTA</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>1295430</t>
+          <t>CGGGGAGGTTTATTTGGCGGAAGGAGGGG</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>1295590</t>
+          <t>CGGGGAGGTTTATTTGGTGGAAGGAGGGG</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>1295680</t>
+          <t>CGGGGCGGTTTCGTCGAGAAAGGGTGGGA</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>1295743</t>
+          <t>CGGGGGATAAGGCGTGTTTTAGGGACGTG</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>1295770</t>
+          <t>CGGGGGATAAGGCGTGTTTTAGGGATGTG</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>1295876</t>
+          <t>CGGGGGTTTGGGTCGCGTTTTTTCGTTCG</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>1295903</t>
+          <t>CGGGGTTAGGGTTTTTTATGTGCGTAGTA</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>1295937</t>
+          <t>CGGGTTTTTAGTTTTTTTGTTATGTGGGA</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>1295979</t>
+          <t>CGGTTGTTGGGGTGATCGTAGTTCGTAGC</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>CGGTTTAGGGGTAGCGTTACGTTTGGGTT</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>CGGTTTTTTTGACGTTATGGTTTTAGGTT</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>CGNAGTGTTTTTTTGTAATATTTTTTCGC</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>CGNGGTTAGGGTTTTTTATGTGCGTAGTA</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>CNGGGCGGTTTCGTCGAGAAAGGGTGGGA</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>CTAAACCACCAACACACAAAAAACCACCA</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>CTAAACCACCAACACACGAAAAACCACCA</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>CTAAACCACCAACGCGCGAAAAACCGCCG</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>CTCCCTAAACGAACACGCGAAACCTCCCA</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>CTCCCTAAACGAACACGCGAAACCTCCCG</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>CTCCCTAAACGAACACGCGAAACCTCNCA</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>GACAACCCTTTAACCGCTAACCTAATCCG</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>GACGACCCTTTAACCGCTAACCTAATCCG</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>GACGACCCTTTAACCGCTAACCTAATNCG</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>TCTATACCCGCGAATCCACTAAAAACCCA</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>TGGAGTGTTTTTTTGTAATATTTTTTTGC</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>TGGCGTAGGTAGGTTCGTACGAAGTCGTA</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGAGGGGTTGGGACGGGGCGGGGTTCG</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGAGGGGTTGGGATGGGGTGGGGTTTG</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGGAGGTTTATTTGGCGGAAGGAGGGG</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGGAGGTTTATTTGGTGGAAGGAGGGG</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGGGTTTGGGTCGCGTTTTTTCGTTCG</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGGTTAGGGTTTTTTATGTGTGTAGTA</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGTTTTCGTGTTGTATTAGTTGTTAGT</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGTTTTTAGTTTTTTCGTTACGTGGGA</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGTTTTTAGTTTTTTTGTTATGTGGGA</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>TGGGTTTTTGTGTTGTATTAGTTGTTAGT</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>TGNAGTGTTTTTTTGTAATATTTTTTTGC</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>TGNGAGGGGTTGGGATGGGGTGGGGTTTG</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>TNGAGTGTTTTTTTGTAATATTTTTTTGC</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>TNGGAGGGGTTGGGATGGGGTGGGGTTTG</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>TNGGGAGGTTTATTTGGTGGAAGGAGGGG</t>
         </is>
       </c>
     </row>
@@ -576,63 +736,65 @@
           <t>SW1710</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0</v>
-      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>